<commit_message>
random order status list tested
</commit_message>
<xml_diff>
--- a/src/test/resources/orderSalesReport.xlsx
+++ b/src/test/resources/orderSalesReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\comag\Documents\Projects\shopeesalescoverter\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6560B733-C6B2-4EF5-8189-4B979981FCF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512BE06A-A3BC-43F9-87C2-21CA9502E94D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="131">
   <si>
     <t>Order ID</t>
   </si>
@@ -749,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BE10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,7 +967,9 @@
       <c r="I2" t="s">
         <v>61</v>
       </c>
-      <c r="J2" s="1"/>
+      <c r="J2" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="K2" t="s">
         <v>62</v>
       </c>
@@ -1132,6 +1134,9 @@
       <c r="I3" t="s">
         <v>61</v>
       </c>
+      <c r="J3" t="s">
+        <v>79</v>
+      </c>
       <c r="K3" t="s">
         <v>62</v>
       </c>
@@ -1293,6 +1298,9 @@
       <c r="I4" t="s">
         <v>61</v>
       </c>
+      <c r="J4" t="s">
+        <v>79</v>
+      </c>
       <c r="K4" t="s">
         <v>62</v>
       </c>
@@ -1453,6 +1461,9 @@
       </c>
       <c r="I5" t="s">
         <v>61</v>
+      </c>
+      <c r="J5" t="s">
+        <v>79</v>
       </c>
       <c r="K5" t="s">
         <v>62</v>

</xml_diff>